<commit_message>
Added OHC user as required for rota meeting
</commit_message>
<xml_diff>
--- a/DaysOff/Rota-08 April 2020.xlsx
+++ b/DaysOff/Rota-08 April 2020.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">  Thursday</t>
   </si>
@@ -50,18 +50,24 @@
     <t xml:space="preserve">  KITCHEN  </t>
   </si>
   <si>
-    <t>MahaDeva</t>
+    <t>MahaDeva PM</t>
   </si>
   <si>
     <t>Navi</t>
   </si>
   <si>
+    <t>MahaDeva - OHC</t>
+  </si>
+  <si>
     <t>Neal</t>
   </si>
   <si>
     <t>Mel</t>
   </si>
   <si>
+    <t>MahaDeva AM</t>
+  </si>
+  <si>
     <t>Adam</t>
   </si>
   <si>
@@ -92,7 +98,7 @@
     <t xml:space="preserve">Rota </t>
   </si>
   <si>
-    <t xml:space="preserve">Mahi Ben Anuka </t>
+    <t xml:space="preserve">MahaDeva Mahi Ben </t>
   </si>
 </sst>
 </file>
@@ -283,7 +289,9 @@
       <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -293,7 +301,7 @@
     <row r="4">
       <c r="A4" s="4"/>
       <c r="B4" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -305,7 +313,7 @@
     <row r="5">
       <c r="A5" s="4"/>
       <c r="B5" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -317,7 +325,7 @@
     <row r="6">
       <c r="A6" s="4"/>
       <c r="B6" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -329,7 +337,7 @@
     <row r="7">
       <c r="A7" s="4"/>
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -341,7 +349,7 @@
     <row r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -353,7 +361,7 @@
     <row r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -365,7 +373,7 @@
     <row r="10">
       <c r="A10" s="4"/>
       <c r="B10" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -377,7 +385,7 @@
     <row r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -389,7 +397,7 @@
     <row r="12">
       <c r="A12" s="4"/>
       <c r="B12" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -400,7 +408,9 @@
     </row>
     <row r="13">
       <c r="A13" s="4"/>
-      <c r="B13" s="7"/>
+      <c r="B13" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -620,16 +630,16 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>